<commit_message>
Outputs de versión 1.3
</commit_message>
<xml_diff>
--- a/Project Outputs for Summits7Beta/BOM Archive/BOM_Summits7Beta.xlsx
+++ b/Project Outputs for Summits7Beta/BOM Archive/BOM_Summits7Beta.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="239">
   <si>
     <t>Component List / BOM Archive</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Version:</t>
   </si>
   <si>
-    <t>Beta 1.0</t>
+    <t>Beta 1.3</t>
   </si>
   <si>
     <t>Website:</t>
@@ -258,7 +258,7 @@
     <t>Ci1</t>
   </si>
   <si>
-    <t>33uF</t>
+    <t>0.1uF</t>
   </si>
   <si>
     <t>19, 20</t>
@@ -464,7 +464,7 @@
     <t>Ra5</t>
   </si>
   <si>
-    <t>5K</t>
+    <t>5.6K</t>
   </si>
   <si>
     <t>36, 37</t>
@@ -497,7 +497,7 @@
     <t>Re1</t>
   </si>
   <si>
-    <t>40.2K</t>
+    <t>43.2K</t>
   </si>
   <si>
     <t>Re2</t>
@@ -699,6 +699,24 @@
   </si>
   <si>
     <t>LM1117MPX-3.3/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>24CW1280T-I/OT</t>
+  </si>
+  <si>
+    <t>EEPROM 128 Kbit I2C</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>579-24CW1280T-I/OT</t>
+  </si>
+  <si>
+    <t>24CW1280T-I/OTCT-ND</t>
   </si>
   <si>
     <t>Y</t>
@@ -2209,7 +2227,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="32">
-        <v>44028.0</v>
+        <v>44069.0</v>
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="34"/>
@@ -4848,33 +4866,33 @@
       <c r="D55" s="89" t="s">
         <v>223</v>
       </c>
-      <c r="E55" s="78" t="s">
+      <c r="E55" s="90" t="s">
         <v>224</v>
       </c>
-      <c r="F55" s="105"/>
-      <c r="G55" s="80">
+      <c r="F55" s="99"/>
+      <c r="G55" s="92">
         <v>1.0</v>
       </c>
-      <c r="H55" s="81" t="s">
+      <c r="H55" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="I55" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="J55" s="95" t="s">
         <v>225</v>
-      </c>
-      <c r="I55" s="82" t="s">
-        <v>34</v>
-      </c>
-      <c r="J55" s="83" t="s">
-        <v>226</v>
       </c>
       <c r="K55" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="L55" s="108" t="s">
-        <v>45</v>
-      </c>
-      <c r="M55" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="N55" s="109" t="s">
-        <v>45</v>
+      <c r="L55" s="94" t="s">
+        <v>37</v>
+      </c>
+      <c r="M55" s="95" t="s">
+        <v>226</v>
+      </c>
+      <c r="N55" s="101" t="s">
+        <v>39</v>
       </c>
       <c r="O55" s="87"/>
       <c r="P55" s="87"/>
@@ -4891,26 +4909,46 @@
       <c r="AA55" s="75"/>
     </row>
     <row r="56">
-      <c r="A56" s="111">
-        <v>24.0</v>
-      </c>
-      <c r="B56" s="112" t="s">
+      <c r="A56" s="76">
+        <v>59.0</v>
+      </c>
+      <c r="B56" s="77" t="s">
         <v>227</v>
       </c>
-      <c r="C56" s="113" t="s">
+      <c r="C56" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="D56" s="114"/>
-      <c r="E56" s="115"/>
-      <c r="F56" s="115"/>
-      <c r="G56" s="115"/>
-      <c r="H56" s="115"/>
-      <c r="I56" s="115"/>
-      <c r="J56" s="115"/>
-      <c r="K56" s="115"/>
-      <c r="L56" s="115"/>
-      <c r="M56" s="115"/>
-      <c r="N56" s="116"/>
+      <c r="D56" s="89" t="s">
+        <v>229</v>
+      </c>
+      <c r="E56" s="78" t="s">
+        <v>230</v>
+      </c>
+      <c r="F56" s="105"/>
+      <c r="G56" s="80">
+        <v>1.0</v>
+      </c>
+      <c r="H56" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="I56" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="J56" s="83" t="s">
+        <v>232</v>
+      </c>
+      <c r="K56" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="L56" s="108" t="s">
+        <v>45</v>
+      </c>
+      <c r="M56" s="92" t="s">
+        <v>45</v>
+      </c>
+      <c r="N56" s="109" t="s">
+        <v>45</v>
+      </c>
       <c r="O56" s="87"/>
       <c r="P56" s="87"/>
       <c r="Q56" s="87"/>
@@ -4926,20 +4964,26 @@
       <c r="AA56" s="75"/>
     </row>
     <row r="57">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
+      <c r="A57" s="111">
+        <v>24.0</v>
+      </c>
+      <c r="B57" s="112" t="s">
+        <v>233</v>
+      </c>
+      <c r="C57" s="113" t="s">
+        <v>234</v>
+      </c>
+      <c r="D57" s="114"/>
+      <c r="E57" s="115"/>
+      <c r="F57" s="115"/>
+      <c r="G57" s="115"/>
+      <c r="H57" s="115"/>
+      <c r="I57" s="115"/>
+      <c r="J57" s="115"/>
+      <c r="K57" s="115"/>
+      <c r="L57" s="115"/>
+      <c r="M57" s="115"/>
+      <c r="N57" s="116"/>
       <c r="O57" s="87"/>
       <c r="P57" s="87"/>
       <c r="Q57" s="87"/>
@@ -4955,16 +4999,12 @@
       <c r="AA57" s="75"/>
     </row>
     <row r="58">
-      <c r="A58" s="117" t="s">
-        <v>229</v>
-      </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="118"/>
-      <c r="D58" s="119" t="s">
-        <v>230</v>
-      </c>
-      <c r="E58" s="37"/>
-      <c r="F58" s="11"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
       <c r="G58" s="18"/>
       <c r="H58" s="18"/>
       <c r="I58" s="18"/>
@@ -4988,11 +5028,13 @@
       <c r="AA58" s="75"/>
     </row>
     <row r="59">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="120"/>
-      <c r="D59" s="121" t="s">
-        <v>231</v>
+      <c r="A59" s="117" t="s">
+        <v>235</v>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="118"/>
+      <c r="D59" s="119" t="s">
+        <v>236</v>
       </c>
       <c r="E59" s="37"/>
       <c r="F59" s="11"/>
@@ -5019,11 +5061,11 @@
       <c r="AA59" s="75"/>
     </row>
     <row r="60">
-      <c r="A60" s="29"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="122"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="120"/>
       <c r="D60" s="121" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E60" s="37"/>
       <c r="F60" s="11"/>
@@ -5050,20 +5092,22 @@
       <c r="AA60" s="75"/>
     </row>
     <row r="61">
-      <c r="A61" s="123"/>
-      <c r="B61" s="124"/>
-      <c r="C61" s="124"/>
-      <c r="D61" s="125"/>
-      <c r="E61" s="126"/>
-      <c r="F61" s="126"/>
-      <c r="G61" s="127"/>
-      <c r="H61" s="127"/>
-      <c r="I61" s="127"/>
-      <c r="J61" s="127"/>
-      <c r="K61" s="127"/>
-      <c r="L61" s="127"/>
-      <c r="M61" s="127"/>
-      <c r="N61" s="127"/>
+      <c r="A61" s="29"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="122"/>
+      <c r="D61" s="121" t="s">
+        <v>238</v>
+      </c>
+      <c r="E61" s="37"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
       <c r="O61" s="87"/>
       <c r="P61" s="87"/>
       <c r="Q61" s="87"/>
@@ -5079,23 +5123,23 @@
       <c r="AA61" s="75"/>
     </row>
     <row r="62">
-      <c r="A62" s="128"/>
-      <c r="B62" s="129"/>
-      <c r="C62" s="129"/>
-      <c r="D62" s="130"/>
-      <c r="E62" s="131"/>
-      <c r="F62" s="131"/>
-      <c r="G62" s="131"/>
-      <c r="H62" s="131"/>
-      <c r="I62" s="131"/>
-      <c r="J62" s="131"/>
-      <c r="K62" s="131"/>
-      <c r="L62" s="131"/>
-      <c r="M62" s="131"/>
-      <c r="N62" s="131"/>
-      <c r="O62" s="131"/>
-      <c r="P62" s="131"/>
-      <c r="Q62" s="131"/>
+      <c r="A62" s="123"/>
+      <c r="B62" s="124"/>
+      <c r="C62" s="124"/>
+      <c r="D62" s="125"/>
+      <c r="E62" s="126"/>
+      <c r="F62" s="126"/>
+      <c r="G62" s="127"/>
+      <c r="H62" s="127"/>
+      <c r="I62" s="127"/>
+      <c r="J62" s="127"/>
+      <c r="K62" s="127"/>
+      <c r="L62" s="127"/>
+      <c r="M62" s="127"/>
+      <c r="N62" s="127"/>
+      <c r="O62" s="87"/>
+      <c r="P62" s="87"/>
+      <c r="Q62" s="87"/>
       <c r="R62" s="87"/>
       <c r="S62" s="74"/>
       <c r="T62" s="74"/>
@@ -5140,7 +5184,7 @@
       <c r="A64" s="128"/>
       <c r="B64" s="129"/>
       <c r="C64" s="129"/>
-      <c r="D64" s="129"/>
+      <c r="D64" s="130"/>
       <c r="E64" s="131"/>
       <c r="F64" s="131"/>
       <c r="G64" s="131"/>
@@ -5166,23 +5210,23 @@
       <c r="AA64" s="75"/>
     </row>
     <row r="65">
-      <c r="A65" s="132"/>
-      <c r="B65" s="133"/>
-      <c r="C65" s="133"/>
-      <c r="D65" s="133"/>
-      <c r="E65" s="87"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="87"/>
-      <c r="H65" s="87"/>
-      <c r="I65" s="87"/>
-      <c r="J65" s="87"/>
-      <c r="K65" s="87"/>
-      <c r="L65" s="87"/>
-      <c r="M65" s="87"/>
-      <c r="N65" s="87"/>
-      <c r="O65" s="87"/>
-      <c r="P65" s="87"/>
-      <c r="Q65" s="87"/>
+      <c r="A65" s="128"/>
+      <c r="B65" s="129"/>
+      <c r="C65" s="129"/>
+      <c r="D65" s="129"/>
+      <c r="E65" s="131"/>
+      <c r="F65" s="131"/>
+      <c r="G65" s="131"/>
+      <c r="H65" s="131"/>
+      <c r="I65" s="131"/>
+      <c r="J65" s="131"/>
+      <c r="K65" s="131"/>
+      <c r="L65" s="131"/>
+      <c r="M65" s="131"/>
+      <c r="N65" s="131"/>
+      <c r="O65" s="131"/>
+      <c r="P65" s="131"/>
+      <c r="Q65" s="131"/>
       <c r="R65" s="87"/>
       <c r="S65" s="74"/>
       <c r="T65" s="74"/>
@@ -5199,25 +5243,25 @@
       <c r="B66" s="133"/>
       <c r="C66" s="133"/>
       <c r="D66" s="133"/>
-      <c r="E66" s="134"/>
-      <c r="F66" s="134"/>
-      <c r="G66" s="134"/>
-      <c r="H66" s="134"/>
-      <c r="I66" s="134"/>
-      <c r="J66" s="134"/>
-      <c r="K66" s="134"/>
-      <c r="L66" s="134"/>
-      <c r="M66" s="134"/>
-      <c r="N66" s="134"/>
-      <c r="O66" s="134"/>
-      <c r="P66" s="134"/>
-      <c r="Q66" s="134"/>
-      <c r="R66" s="134"/>
-      <c r="S66" s="135"/>
-      <c r="T66" s="135"/>
-      <c r="U66" s="135"/>
-      <c r="V66" s="135"/>
-      <c r="W66" s="135"/>
+      <c r="E66" s="87"/>
+      <c r="F66" s="87"/>
+      <c r="G66" s="87"/>
+      <c r="H66" s="87"/>
+      <c r="I66" s="87"/>
+      <c r="J66" s="87"/>
+      <c r="K66" s="87"/>
+      <c r="L66" s="87"/>
+      <c r="M66" s="87"/>
+      <c r="N66" s="87"/>
+      <c r="O66" s="87"/>
+      <c r="P66" s="87"/>
+      <c r="Q66" s="87"/>
+      <c r="R66" s="87"/>
+      <c r="S66" s="74"/>
+      <c r="T66" s="74"/>
+      <c r="U66" s="74"/>
+      <c r="V66" s="74"/>
+      <c r="W66" s="74"/>
       <c r="X66" s="75"/>
       <c r="Y66" s="75"/>
       <c r="Z66" s="75"/>
@@ -5227,7 +5271,7 @@
       <c r="A67" s="132"/>
       <c r="B67" s="133"/>
       <c r="C67" s="133"/>
-      <c r="D67" s="46"/>
+      <c r="D67" s="133"/>
       <c r="E67" s="134"/>
       <c r="F67" s="134"/>
       <c r="G67" s="134"/>
@@ -5256,7 +5300,7 @@
       <c r="A68" s="132"/>
       <c r="B68" s="133"/>
       <c r="C68" s="133"/>
-      <c r="D68" s="133"/>
+      <c r="D68" s="46"/>
       <c r="E68" s="134"/>
       <c r="F68" s="134"/>
       <c r="G68" s="134"/>
@@ -5284,7 +5328,7 @@
     <row r="69">
       <c r="A69" s="132"/>
       <c r="B69" s="133"/>
-      <c r="C69" s="132"/>
+      <c r="C69" s="133"/>
       <c r="D69" s="133"/>
       <c r="E69" s="134"/>
       <c r="F69" s="134"/>
@@ -5340,9 +5384,9 @@
       <c r="AA70" s="75"/>
     </row>
     <row r="71">
-      <c r="A71" s="133"/>
+      <c r="A71" s="132"/>
       <c r="B71" s="133"/>
-      <c r="C71" s="133"/>
+      <c r="C71" s="132"/>
       <c r="D71" s="133"/>
       <c r="E71" s="134"/>
       <c r="F71" s="134"/>
@@ -5369,7 +5413,7 @@
       <c r="AA71" s="75"/>
     </row>
     <row r="72">
-      <c r="A72" s="132"/>
+      <c r="A72" s="133"/>
       <c r="B72" s="133"/>
       <c r="C72" s="133"/>
       <c r="D72" s="133"/>
@@ -5398,7 +5442,7 @@
       <c r="AA72" s="75"/>
     </row>
     <row r="73">
-      <c r="A73" s="133"/>
+      <c r="A73" s="132"/>
       <c r="B73" s="133"/>
       <c r="C73" s="133"/>
       <c r="D73" s="133"/>
@@ -5427,7 +5471,7 @@
       <c r="AA73" s="75"/>
     </row>
     <row r="74">
-      <c r="A74" s="132"/>
+      <c r="A74" s="133"/>
       <c r="B74" s="133"/>
       <c r="C74" s="133"/>
       <c r="D74" s="133"/>
@@ -5488,7 +5532,7 @@
       <c r="A76" s="132"/>
       <c r="B76" s="133"/>
       <c r="C76" s="133"/>
-      <c r="D76" s="46"/>
+      <c r="D76" s="133"/>
       <c r="E76" s="134"/>
       <c r="F76" s="134"/>
       <c r="G76" s="134"/>
@@ -5517,7 +5561,7 @@
       <c r="A77" s="132"/>
       <c r="B77" s="133"/>
       <c r="C77" s="133"/>
-      <c r="D77" s="133"/>
+      <c r="D77" s="46"/>
       <c r="E77" s="134"/>
       <c r="F77" s="134"/>
       <c r="G77" s="134"/>
@@ -5603,7 +5647,7 @@
     <row r="80">
       <c r="A80" s="132"/>
       <c r="B80" s="133"/>
-      <c r="C80" s="132"/>
+      <c r="C80" s="133"/>
       <c r="D80" s="133"/>
       <c r="E80" s="134"/>
       <c r="F80" s="134"/>
@@ -5630,6 +5674,10 @@
       <c r="AA80" s="75"/>
     </row>
     <row r="81">
+      <c r="A81" s="132"/>
+      <c r="B81" s="133"/>
+      <c r="C81" s="132"/>
+      <c r="D81" s="133"/>
       <c r="E81" s="134"/>
       <c r="F81" s="134"/>
       <c r="G81" s="134"/>
@@ -5655,10 +5703,6 @@
       <c r="AA81" s="75"/>
     </row>
     <row r="82">
-      <c r="A82" s="132"/>
-      <c r="B82" s="133"/>
-      <c r="C82" s="133"/>
-      <c r="D82" s="133"/>
       <c r="E82" s="134"/>
       <c r="F82" s="134"/>
       <c r="G82" s="134"/>
@@ -5745,7 +5789,7 @@
       <c r="A85" s="132"/>
       <c r="B85" s="133"/>
       <c r="C85" s="133"/>
-      <c r="D85" s="46"/>
+      <c r="D85" s="133"/>
       <c r="E85" s="134"/>
       <c r="F85" s="134"/>
       <c r="G85" s="134"/>
@@ -5774,7 +5818,7 @@
       <c r="A86" s="132"/>
       <c r="B86" s="133"/>
       <c r="C86" s="133"/>
-      <c r="D86" s="133"/>
+      <c r="D86" s="46"/>
       <c r="E86" s="134"/>
       <c r="F86" s="134"/>
       <c r="G86" s="134"/>
@@ -5858,10 +5902,10 @@
       <c r="AA88" s="75"/>
     </row>
     <row r="89">
-      <c r="A89" s="134"/>
-      <c r="B89" s="134"/>
-      <c r="C89" s="134"/>
-      <c r="D89" s="134"/>
+      <c r="A89" s="132"/>
+      <c r="B89" s="133"/>
+      <c r="C89" s="133"/>
+      <c r="D89" s="133"/>
       <c r="E89" s="134"/>
       <c r="F89" s="134"/>
       <c r="G89" s="134"/>
@@ -5887,29 +5931,33 @@
       <c r="AA89" s="75"/>
     </row>
     <row r="90">
-      <c r="A90" s="136"/>
-      <c r="B90" s="136"/>
-      <c r="C90" s="136"/>
-      <c r="D90" s="136"/>
-      <c r="E90" s="136"/>
-      <c r="F90" s="136"/>
-      <c r="G90" s="136"/>
-      <c r="H90" s="136"/>
-      <c r="I90" s="136"/>
-      <c r="J90" s="136"/>
-      <c r="K90" s="136"/>
-      <c r="L90" s="136"/>
-      <c r="M90" s="136"/>
-      <c r="N90" s="136"/>
-      <c r="O90" s="136"/>
-      <c r="P90" s="136"/>
-      <c r="Q90" s="136"/>
-      <c r="R90" s="136"/>
-      <c r="S90" s="137"/>
-      <c r="T90" s="137"/>
-      <c r="U90" s="137"/>
-      <c r="V90" s="137"/>
-      <c r="W90" s="137"/>
+      <c r="A90" s="134"/>
+      <c r="B90" s="134"/>
+      <c r="C90" s="134"/>
+      <c r="D90" s="134"/>
+      <c r="E90" s="134"/>
+      <c r="F90" s="134"/>
+      <c r="G90" s="134"/>
+      <c r="H90" s="134"/>
+      <c r="I90" s="134"/>
+      <c r="J90" s="134"/>
+      <c r="K90" s="134"/>
+      <c r="L90" s="134"/>
+      <c r="M90" s="134"/>
+      <c r="N90" s="134"/>
+      <c r="O90" s="134"/>
+      <c r="P90" s="134"/>
+      <c r="Q90" s="134"/>
+      <c r="R90" s="134"/>
+      <c r="S90" s="135"/>
+      <c r="T90" s="135"/>
+      <c r="U90" s="135"/>
+      <c r="V90" s="135"/>
+      <c r="W90" s="135"/>
+      <c r="X90" s="75"/>
+      <c r="Y90" s="75"/>
+      <c r="Z90" s="75"/>
+      <c r="AA90" s="75"/>
     </row>
     <row r="91">
       <c r="A91" s="136"/>
@@ -6062,24 +6110,29 @@
       <c r="W96" s="137"/>
     </row>
     <row r="97">
-      <c r="A97" s="138"/>
-      <c r="B97" s="138"/>
-      <c r="C97" s="138"/>
-      <c r="D97" s="138"/>
-      <c r="E97" s="138"/>
-      <c r="F97" s="138"/>
-      <c r="G97" s="138"/>
-      <c r="H97" s="138"/>
-      <c r="I97" s="138"/>
-      <c r="J97" s="138"/>
-      <c r="K97" s="138"/>
-      <c r="L97" s="138"/>
-      <c r="M97" s="138"/>
-      <c r="N97" s="138"/>
-      <c r="O97" s="138"/>
-      <c r="P97" s="138"/>
-      <c r="Q97" s="138"/>
-      <c r="R97" s="138"/>
+      <c r="A97" s="136"/>
+      <c r="B97" s="136"/>
+      <c r="C97" s="136"/>
+      <c r="D97" s="136"/>
+      <c r="E97" s="136"/>
+      <c r="F97" s="136"/>
+      <c r="G97" s="136"/>
+      <c r="H97" s="136"/>
+      <c r="I97" s="136"/>
+      <c r="J97" s="136"/>
+      <c r="K97" s="136"/>
+      <c r="L97" s="136"/>
+      <c r="M97" s="136"/>
+      <c r="N97" s="136"/>
+      <c r="O97" s="136"/>
+      <c r="P97" s="136"/>
+      <c r="Q97" s="136"/>
+      <c r="R97" s="136"/>
+      <c r="S97" s="137"/>
+      <c r="T97" s="137"/>
+      <c r="U97" s="137"/>
+      <c r="V97" s="137"/>
+      <c r="W97" s="137"/>
     </row>
     <row r="98">
       <c r="A98" s="138"/>
@@ -6681,6 +6734,26 @@
       <c r="Q127" s="138"/>
       <c r="R127" s="138"/>
     </row>
+    <row r="128">
+      <c r="A128" s="138"/>
+      <c r="B128" s="138"/>
+      <c r="C128" s="138"/>
+      <c r="D128" s="138"/>
+      <c r="E128" s="138"/>
+      <c r="F128" s="138"/>
+      <c r="G128" s="138"/>
+      <c r="H128" s="138"/>
+      <c r="I128" s="138"/>
+      <c r="J128" s="138"/>
+      <c r="K128" s="138"/>
+      <c r="L128" s="138"/>
+      <c r="M128" s="138"/>
+      <c r="N128" s="138"/>
+      <c r="O128" s="138"/>
+      <c r="P128" s="138"/>
+      <c r="Q128" s="138"/>
+      <c r="R128" s="138"/>
+    </row>
   </sheetData>
   <mergeCells count="26">
     <mergeCell ref="F4:G4"/>
@@ -6699,16 +6772,16 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D58:F58"/>
     <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="D56:N56"/>
-    <mergeCell ref="A58:B60"/>
-    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D57:N57"/>
+    <mergeCell ref="A59:B61"/>
+    <mergeCell ref="D61:F61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H4"/>
@@ -6744,10 +6817,12 @@
     <hyperlink r:id="rId31" ref="K54"/>
     <hyperlink r:id="rId32" ref="N54"/>
     <hyperlink r:id="rId33" ref="K55"/>
+    <hyperlink r:id="rId34" ref="N55"/>
+    <hyperlink r:id="rId35" ref="K56"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId34"/>
+  <drawing r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>